<commit_message>
ultimo commit extra con documentación y arreglos añadidos
</commit_message>
<xml_diff>
--- a/Documentacion/Tokens.xlsx
+++ b/Documentacion/Tokens.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="42">
   <si>
     <t>Tokens</t>
   </si>
@@ -115,13 +115,43 @@
   </si>
   <si>
     <t>exportarReporte</t>
+  </si>
+  <si>
+    <t>TITULO</t>
+  </si>
+  <si>
+    <t>Token</t>
+  </si>
+  <si>
+    <t>Lexema</t>
+  </si>
+  <si>
+    <t>Patrón</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>Le = [A_Z, a_z] -&gt; Palabra = Le+ -&gt; "palabra"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Di = [0_9] -&gt; Digito = (-)?Di+(.Di+)? -&gt; Digito </t>
+  </si>
+  <si>
+    <t>Let = [A_Z, a_z,\t, _] -&gt; #(Let)*(\n)</t>
+  </si>
+  <si>
+    <t>LeT = [A_Z, a_z, \n, \t, \r, _] -&gt; ‘’’(LeT)*‘’’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conteo </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,16 +167,65 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE699"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBDD7EE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6E0B4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD966"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8EA9DB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA9D08E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -154,11 +233,185 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -167,6 +420,42 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -449,24 +738,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="24.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="49.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -474,7 +766,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -482,7 +774,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -490,7 +782,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -498,7 +790,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -506,7 +798,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -514,156 +806,404 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E8" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E9" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E21" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E22" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E23" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E24" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E25" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>2</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E27" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E28" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E29" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E30" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E31" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E32" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E33" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>